<commit_message>
support tournament of 32
</commit_message>
<xml_diff>
--- a/templates/tmpl_tournament.xlsx
+++ b/templates/tmpl_tournament.xlsx
@@ -5,25 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoyagi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoyagi/work/tkd/tkd_competition_manager/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5BF0D9-31E1-294B-8179-DEDBC83CA3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0DBD9C-6362-0745-9BEA-7A1DD1D1DEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23020" yWindow="2420" windowWidth="31280" windowHeight="35960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2" sheetId="7" r:id="rId1"/>
     <sheet name="4" sheetId="2" r:id="rId2"/>
     <sheet name="8" sheetId="1" r:id="rId3"/>
     <sheet name="16" sheetId="11" r:id="rId4"/>
+    <sheet name="32" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49,7 +46,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -130,11 +127,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -143,6 +180,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -3638,7 +3679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
@@ -4837,4 +4878,1464 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB5529E-DB6E-8C48-B455-FE5C1AE79309}">
+  <dimension ref="A1:F1002"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="23" width="7.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:6" ht="3.75" customHeight="1"/>
+    <row r="2" spans="4:6" ht="16.5" customHeight="1"/>
+    <row r="3" spans="4:6" ht="16.5" customHeight="1">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="4:6" ht="3.75" customHeight="1">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="4:6" ht="3.75" customHeight="1">
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="4:6" ht="16.5" customHeight="1">
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="4:6" ht="16.5" customHeight="1">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="4:6" ht="3.75" customHeight="1">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="4:6" ht="3.75" customHeight="1">
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="4:6" ht="16.5" customHeight="1">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="4:6" ht="16.5" customHeight="1">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="4:6" ht="3.75" customHeight="1">
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="4:6" ht="3.75" customHeight="1">
+      <c r="D13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="4:6" ht="16.5" customHeight="1">
+      <c r="D14" s="2"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="4:6" ht="16.5" customHeight="1">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="4:6" ht="3.75" customHeight="1">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="3:6" ht="3.75" customHeight="1">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="3:6" ht="16.5" customHeight="1">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="3:6" ht="16.5" customHeight="1">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="3:6" ht="3.75" customHeight="1">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="3:6" ht="3.75" customHeight="1">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="3:6" ht="16.5" customHeight="1">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="3:6" ht="16.5" customHeight="1">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="3:6" ht="3.75" customHeight="1">
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="3:6" ht="3.75" customHeight="1">
+      <c r="C25" s="2"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="3:6" ht="16.5" customHeight="1">
+      <c r="C26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="3:6" ht="16.5" customHeight="1">
+      <c r="C27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="3:6" ht="3.75" customHeight="1">
+      <c r="C28" s="2"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="3:6" ht="3.75" customHeight="1">
+      <c r="C29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="3:6" ht="16.5" customHeight="1">
+      <c r="C30" s="2"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="3:6" ht="16.5" customHeight="1">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="3:6" ht="3.75" customHeight="1">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B34" s="8"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B35" s="8"/>
+      <c r="C35" s="2"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B36" s="8"/>
+      <c r="C36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B37" s="8"/>
+      <c r="C37" s="2"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B38" s="8"/>
+      <c r="C38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B39" s="8"/>
+      <c r="C39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B40" s="8"/>
+      <c r="C40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B41" s="8"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B42" s="8"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B43" s="8"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B44" s="8"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B45" s="8"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B46" s="8"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B47" s="8"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B48" s="8"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B49" s="8"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B50" s="8"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B51" s="8"/>
+      <c r="D51" s="2"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B52" s="8"/>
+      <c r="D52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B53" s="8"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B54" s="8"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B55" s="8"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B56" s="8"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B57" s="8"/>
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B58" s="8"/>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B59" s="8"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B60" s="8"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B61" s="8"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B62" s="8"/>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B63" s="8"/>
+    </row>
+    <row r="64" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B64" s="8"/>
+    </row>
+    <row r="65" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A65" s="10"/>
+      <c r="B65" s="8"/>
+    </row>
+    <row r="66" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A66" s="11"/>
+    </row>
+    <row r="67" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B67" s="8"/>
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:6" ht="3.75" customHeight="1">
+      <c r="B68" s="8"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" ht="3.75" customHeight="1">
+      <c r="B69" s="8"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B70" s="8"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B71" s="8"/>
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" ht="3.75" customHeight="1">
+      <c r="B72" s="8"/>
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" ht="3.75" customHeight="1">
+      <c r="B73" s="8"/>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B74" s="8"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B75" s="8"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76" spans="1:6" ht="3.75" customHeight="1">
+      <c r="B76" s="8"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" ht="3.75" customHeight="1">
+      <c r="B77" s="8"/>
+      <c r="D77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B78" s="8"/>
+      <c r="D78" s="2"/>
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B79" s="8"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" ht="3.75" customHeight="1">
+      <c r="B80" s="8"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B81" s="8"/>
+      <c r="C81" s="5"/>
+    </row>
+    <row r="82" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B82" s="8"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B83" s="8"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="F83" s="1"/>
+    </row>
+    <row r="84" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B84" s="8"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B85" s="8"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B86" s="8"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="3"/>
+    </row>
+    <row r="87" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B87" s="8"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B88" s="8"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="2"/>
+    </row>
+    <row r="89" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B89" s="8"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="7"/>
+    </row>
+    <row r="90" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B90" s="8"/>
+      <c r="C90" s="2"/>
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B91" s="8"/>
+      <c r="C91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="1"/>
+    </row>
+    <row r="92" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B92" s="8"/>
+      <c r="C92" s="2"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B93" s="8"/>
+      <c r="C93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B94" s="8"/>
+      <c r="C94" s="2"/>
+      <c r="F94" s="3"/>
+    </row>
+    <row r="95" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B95" s="8"/>
+      <c r="C95" s="2"/>
+    </row>
+    <row r="96" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B96" s="9"/>
+      <c r="C96" s="2"/>
+    </row>
+    <row r="97" spans="2:6" ht="3.75" customHeight="1">
+      <c r="B97" s="6"/>
+    </row>
+    <row r="98" spans="2:6" ht="16.5" customHeight="1">
+      <c r="C98" s="2"/>
+    </row>
+    <row r="99" spans="2:6" ht="16.5" customHeight="1">
+      <c r="C99" s="2"/>
+      <c r="F99" s="1"/>
+    </row>
+    <row r="100" spans="2:6" ht="3.75" customHeight="1">
+      <c r="C100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="2:6" ht="3.75" customHeight="1">
+      <c r="C101" s="2"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="2:6" ht="16.5" customHeight="1">
+      <c r="C102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="2:6" ht="16.5" customHeight="1">
+      <c r="C103" s="2"/>
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="2:6" ht="3.75" customHeight="1">
+      <c r="C104" s="2"/>
+      <c r="E104" s="2"/>
+    </row>
+    <row r="105" spans="2:6" ht="3.75" customHeight="1">
+      <c r="C105" s="2"/>
+      <c r="D105" s="5"/>
+    </row>
+    <row r="106" spans="2:6" ht="16.5" customHeight="1">
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+    </row>
+    <row r="107" spans="2:6" ht="16.5" customHeight="1">
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="1"/>
+    </row>
+    <row r="108" spans="2:6" ht="3.75" customHeight="1">
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="2"/>
+    </row>
+    <row r="109" spans="2:6" ht="3.75" customHeight="1">
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="F109" s="2"/>
+    </row>
+    <row r="110" spans="2:6" ht="16.5" customHeight="1">
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="F110" s="3"/>
+    </row>
+    <row r="111" spans="2:6" ht="16.5" customHeight="1">
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+    </row>
+    <row r="112" spans="2:6" ht="3.75" customHeight="1">
+      <c r="C112" s="3"/>
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="4:6" ht="3.75" customHeight="1">
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="4:6" ht="16.5" customHeight="1">
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115" spans="4:6" ht="16.5" customHeight="1">
+      <c r="D115" s="2"/>
+      <c r="F115" s="1"/>
+    </row>
+    <row r="116" spans="4:6" ht="3.75" customHeight="1">
+      <c r="D116" s="2"/>
+      <c r="F116" s="2"/>
+    </row>
+    <row r="117" spans="4:6" ht="3.75" customHeight="1">
+      <c r="D117" s="2"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="2"/>
+    </row>
+    <row r="118" spans="4:6" ht="16.5" customHeight="1">
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="3"/>
+    </row>
+    <row r="119" spans="4:6" ht="16.5" customHeight="1">
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+    </row>
+    <row r="120" spans="4:6" ht="3.75" customHeight="1">
+      <c r="D120" s="3"/>
+      <c r="E120" s="2"/>
+    </row>
+    <row r="121" spans="4:6" ht="3.75" customHeight="1">
+      <c r="D121" s="7"/>
+    </row>
+    <row r="122" spans="4:6" ht="16.5" customHeight="1">
+      <c r="E122" s="2"/>
+    </row>
+    <row r="123" spans="4:6" ht="16.5" customHeight="1">
+      <c r="E123" s="2"/>
+      <c r="F123" s="1"/>
+    </row>
+    <row r="124" spans="4:6" ht="3.75" customHeight="1">
+      <c r="E124" s="3"/>
+      <c r="F124" s="2"/>
+    </row>
+    <row r="125" spans="4:6" ht="3.75" customHeight="1">
+      <c r="F125" s="2"/>
+    </row>
+    <row r="126" spans="4:6" ht="16.5" customHeight="1">
+      <c r="F126" s="3"/>
+    </row>
+    <row r="127" spans="4:6" ht="16.5" customHeight="1"/>
+    <row r="128" spans="4:6" ht="16.5" customHeight="1"/>
+    <row r="129" ht="16.5" customHeight="1"/>
+    <row r="130" ht="16.5" customHeight="1"/>
+    <row r="131" ht="16.5" customHeight="1"/>
+    <row r="132" ht="16.5" customHeight="1"/>
+    <row r="133" ht="16.5" customHeight="1"/>
+    <row r="134" ht="16.5" customHeight="1"/>
+    <row r="135" ht="16.5" customHeight="1"/>
+    <row r="136" ht="16.5" customHeight="1"/>
+    <row r="137" ht="16.5" customHeight="1"/>
+    <row r="138" ht="16.5" customHeight="1"/>
+    <row r="139" ht="16.5" customHeight="1"/>
+    <row r="140" ht="16.5" customHeight="1"/>
+    <row r="141" ht="16.5" customHeight="1"/>
+    <row r="142" ht="16.5" customHeight="1"/>
+    <row r="143" ht="16.5" customHeight="1"/>
+    <row r="144" ht="16.5" customHeight="1"/>
+    <row r="145" ht="16.5" customHeight="1"/>
+    <row r="146" ht="16.5" customHeight="1"/>
+    <row r="147" ht="16.5" customHeight="1"/>
+    <row r="148" ht="16.5" customHeight="1"/>
+    <row r="149" ht="16.5" customHeight="1"/>
+    <row r="150" ht="16.5" customHeight="1"/>
+    <row r="151" ht="16.5" customHeight="1"/>
+    <row r="152" ht="16.5" customHeight="1"/>
+    <row r="153" ht="16.5" customHeight="1"/>
+    <row r="154" ht="16.5" customHeight="1"/>
+    <row r="155" ht="16.5" customHeight="1"/>
+    <row r="156" ht="16.5" customHeight="1"/>
+    <row r="157" ht="16.5" customHeight="1"/>
+    <row r="158" ht="16.5" customHeight="1"/>
+    <row r="159" ht="16.5" customHeight="1"/>
+    <row r="160" ht="16.5" customHeight="1"/>
+    <row r="161" ht="16.5" customHeight="1"/>
+    <row r="162" ht="16.5" customHeight="1"/>
+    <row r="163" ht="16.5" customHeight="1"/>
+    <row r="164" ht="16.5" customHeight="1"/>
+    <row r="165" ht="16.5" customHeight="1"/>
+    <row r="166" ht="16.5" customHeight="1"/>
+    <row r="167" ht="16.5" customHeight="1"/>
+    <row r="168" ht="16.5" customHeight="1"/>
+    <row r="169" ht="16.5" customHeight="1"/>
+    <row r="170" ht="16.5" customHeight="1"/>
+    <row r="171" ht="16.5" customHeight="1"/>
+    <row r="172" ht="16.5" customHeight="1"/>
+    <row r="173" ht="16.5" customHeight="1"/>
+    <row r="174" ht="16.5" customHeight="1"/>
+    <row r="175" ht="16.5" customHeight="1"/>
+    <row r="176" ht="16.5" customHeight="1"/>
+    <row r="177" ht="16.5" customHeight="1"/>
+    <row r="178" ht="16.5" customHeight="1"/>
+    <row r="179" ht="16.5" customHeight="1"/>
+    <row r="180" ht="16.5" customHeight="1"/>
+    <row r="181" ht="16.5" customHeight="1"/>
+    <row r="182" ht="16.5" customHeight="1"/>
+    <row r="183" ht="16.5" customHeight="1"/>
+    <row r="184" ht="16.5" customHeight="1"/>
+    <row r="185" ht="16.5" customHeight="1"/>
+    <row r="186" ht="16.5" customHeight="1"/>
+    <row r="187" ht="16.5" customHeight="1"/>
+    <row r="188" ht="16.5" customHeight="1"/>
+    <row r="189" ht="16.5" customHeight="1"/>
+    <row r="190" ht="16.5" customHeight="1"/>
+    <row r="191" ht="16.5" customHeight="1"/>
+    <row r="192" ht="16.5" customHeight="1"/>
+    <row r="193" ht="16.5" customHeight="1"/>
+    <row r="194" ht="16.5" customHeight="1"/>
+    <row r="195" ht="16.5" customHeight="1"/>
+    <row r="196" ht="16.5" customHeight="1"/>
+    <row r="197" ht="16.5" customHeight="1"/>
+    <row r="198" ht="16.5" customHeight="1"/>
+    <row r="199" ht="16.5" customHeight="1"/>
+    <row r="200" ht="16.5" customHeight="1"/>
+    <row r="201" ht="16.5" customHeight="1"/>
+    <row r="202" ht="16.5" customHeight="1"/>
+    <row r="203" ht="16.5" customHeight="1"/>
+    <row r="204" ht="16.5" customHeight="1"/>
+    <row r="205" ht="16.5" customHeight="1"/>
+    <row r="206" ht="16.5" customHeight="1"/>
+    <row r="207" ht="16.5" customHeight="1"/>
+    <row r="208" ht="16.5" customHeight="1"/>
+    <row r="209" ht="16.5" customHeight="1"/>
+    <row r="210" ht="16.5" customHeight="1"/>
+    <row r="211" ht="16.5" customHeight="1"/>
+    <row r="212" ht="16.5" customHeight="1"/>
+    <row r="213" ht="16.5" customHeight="1"/>
+    <row r="214" ht="16.5" customHeight="1"/>
+    <row r="215" ht="16.5" customHeight="1"/>
+    <row r="216" ht="16.5" customHeight="1"/>
+    <row r="217" ht="16.5" customHeight="1"/>
+    <row r="218" ht="16.5" customHeight="1"/>
+    <row r="219" ht="16.5" customHeight="1"/>
+    <row r="220" ht="16.5" customHeight="1"/>
+    <row r="221" ht="16.5" customHeight="1"/>
+    <row r="222" ht="16.5" customHeight="1"/>
+    <row r="223" ht="16.5" customHeight="1"/>
+    <row r="224" ht="16.5" customHeight="1"/>
+    <row r="225" ht="16.5" customHeight="1"/>
+    <row r="226" ht="16.5" customHeight="1"/>
+    <row r="227" ht="16.5" customHeight="1"/>
+    <row r="228" ht="16.5" customHeight="1"/>
+    <row r="229" ht="16.5" customHeight="1"/>
+    <row r="230" ht="16.5" customHeight="1"/>
+    <row r="231" ht="16.5" customHeight="1"/>
+    <row r="232" ht="16.5" customHeight="1"/>
+    <row r="233" ht="16.5" customHeight="1"/>
+    <row r="234" ht="16.5" customHeight="1"/>
+    <row r="235" ht="16.5" customHeight="1"/>
+    <row r="236" ht="16.5" customHeight="1"/>
+    <row r="237" ht="16.5" customHeight="1"/>
+    <row r="238" ht="16.5" customHeight="1"/>
+    <row r="239" ht="16.5" customHeight="1"/>
+    <row r="240" ht="16.5" customHeight="1"/>
+    <row r="241" ht="16.5" customHeight="1"/>
+    <row r="242" ht="16.5" customHeight="1"/>
+    <row r="243" ht="16.5" customHeight="1"/>
+    <row r="244" ht="16.5" customHeight="1"/>
+    <row r="245" ht="16.5" customHeight="1"/>
+    <row r="246" ht="16.5" customHeight="1"/>
+    <row r="247" ht="16.5" customHeight="1"/>
+    <row r="248" ht="16.5" customHeight="1"/>
+    <row r="249" ht="16.5" customHeight="1"/>
+    <row r="250" ht="16.5" customHeight="1"/>
+    <row r="251" ht="16.5" customHeight="1"/>
+    <row r="252" ht="16.5" customHeight="1"/>
+    <row r="253" ht="16.5" customHeight="1"/>
+    <row r="254" ht="16.5" customHeight="1"/>
+    <row r="255" ht="16.5" customHeight="1"/>
+    <row r="256" ht="16.5" customHeight="1"/>
+    <row r="257" ht="16.5" customHeight="1"/>
+    <row r="258" ht="16.5" customHeight="1"/>
+    <row r="259" ht="16.5" customHeight="1"/>
+    <row r="260" ht="16.5" customHeight="1"/>
+    <row r="261" ht="16.5" customHeight="1"/>
+    <row r="262" ht="16.5" customHeight="1"/>
+    <row r="263" ht="16.5" customHeight="1"/>
+    <row r="264" ht="16.5" customHeight="1"/>
+    <row r="265" ht="16.5" customHeight="1"/>
+    <row r="266" ht="16.5" customHeight="1"/>
+    <row r="267" ht="16.5" customHeight="1"/>
+    <row r="268" ht="16.5" customHeight="1"/>
+    <row r="269" ht="16.5" customHeight="1"/>
+    <row r="270" ht="16.5" customHeight="1"/>
+    <row r="271" ht="16.5" customHeight="1"/>
+    <row r="272" ht="16.5" customHeight="1"/>
+    <row r="273" ht="16.5" customHeight="1"/>
+    <row r="274" ht="16.5" customHeight="1"/>
+    <row r="275" ht="16.5" customHeight="1"/>
+    <row r="276" ht="16.5" customHeight="1"/>
+    <row r="277" ht="16.5" customHeight="1"/>
+    <row r="278" ht="16.5" customHeight="1"/>
+    <row r="279" ht="16.5" customHeight="1"/>
+    <row r="280" ht="16.5" customHeight="1"/>
+    <row r="281" ht="16.5" customHeight="1"/>
+    <row r="282" ht="16.5" customHeight="1"/>
+    <row r="283" ht="16.5" customHeight="1"/>
+    <row r="284" ht="16.5" customHeight="1"/>
+    <row r="285" ht="16.5" customHeight="1"/>
+    <row r="286" ht="16.5" customHeight="1"/>
+    <row r="287" ht="16.5" customHeight="1"/>
+    <row r="288" ht="16.5" customHeight="1"/>
+    <row r="289" ht="16.5" customHeight="1"/>
+    <row r="290" ht="16.5" customHeight="1"/>
+    <row r="291" ht="16.5" customHeight="1"/>
+    <row r="292" ht="16.5" customHeight="1"/>
+    <row r="293" ht="16.5" customHeight="1"/>
+    <row r="294" ht="16.5" customHeight="1"/>
+    <row r="295" ht="16.5" customHeight="1"/>
+    <row r="296" ht="16.5" customHeight="1"/>
+    <row r="297" ht="16.5" customHeight="1"/>
+    <row r="298" ht="16.5" customHeight="1"/>
+    <row r="299" ht="16.5" customHeight="1"/>
+    <row r="300" ht="16.5" customHeight="1"/>
+    <row r="301" ht="16.5" customHeight="1"/>
+    <row r="302" ht="16.5" customHeight="1"/>
+    <row r="303" ht="16.5" customHeight="1"/>
+    <row r="304" ht="16.5" customHeight="1"/>
+    <row r="305" ht="16.5" customHeight="1"/>
+    <row r="306" ht="16.5" customHeight="1"/>
+    <row r="307" ht="16.5" customHeight="1"/>
+    <row r="308" ht="16.5" customHeight="1"/>
+    <row r="309" ht="16.5" customHeight="1"/>
+    <row r="310" ht="16.5" customHeight="1"/>
+    <row r="311" ht="16.5" customHeight="1"/>
+    <row r="312" ht="16.5" customHeight="1"/>
+    <row r="313" ht="16.5" customHeight="1"/>
+    <row r="314" ht="16.5" customHeight="1"/>
+    <row r="315" ht="16.5" customHeight="1"/>
+    <row r="316" ht="16.5" customHeight="1"/>
+    <row r="317" ht="16.5" customHeight="1"/>
+    <row r="318" ht="16.5" customHeight="1"/>
+    <row r="319" ht="16.5" customHeight="1"/>
+    <row r="320" ht="16.5" customHeight="1"/>
+    <row r="321" ht="16.5" customHeight="1"/>
+    <row r="322" ht="16.5" customHeight="1"/>
+    <row r="323" ht="16.5" customHeight="1"/>
+    <row r="324" ht="16.5" customHeight="1"/>
+    <row r="325" ht="16.5" customHeight="1"/>
+    <row r="326" ht="16.5" customHeight="1"/>
+    <row r="327" ht="16.5" customHeight="1"/>
+    <row r="328" ht="16.5" customHeight="1"/>
+    <row r="329" ht="16.5" customHeight="1"/>
+    <row r="330" ht="16.5" customHeight="1"/>
+    <row r="331" ht="16.5" customHeight="1"/>
+    <row r="332" ht="16.5" customHeight="1"/>
+    <row r="333" ht="16.5" customHeight="1"/>
+    <row r="334" ht="16.5" customHeight="1"/>
+    <row r="335" ht="16.5" customHeight="1"/>
+    <row r="336" ht="16.5" customHeight="1"/>
+    <row r="337" ht="16.5" customHeight="1"/>
+    <row r="338" ht="16.5" customHeight="1"/>
+    <row r="339" ht="16.5" customHeight="1"/>
+    <row r="340" ht="16.5" customHeight="1"/>
+    <row r="341" ht="16.5" customHeight="1"/>
+    <row r="342" ht="16.5" customHeight="1"/>
+    <row r="343" ht="16.5" customHeight="1"/>
+    <row r="344" ht="16.5" customHeight="1"/>
+    <row r="345" ht="16.5" customHeight="1"/>
+    <row r="346" ht="16.5" customHeight="1"/>
+    <row r="347" ht="16.5" customHeight="1"/>
+    <row r="348" ht="16.5" customHeight="1"/>
+    <row r="349" ht="16.5" customHeight="1"/>
+    <row r="350" ht="16.5" customHeight="1"/>
+    <row r="351" ht="16.5" customHeight="1"/>
+    <row r="352" ht="16.5" customHeight="1"/>
+    <row r="353" ht="16.5" customHeight="1"/>
+    <row r="354" ht="16.5" customHeight="1"/>
+    <row r="355" ht="16.5" customHeight="1"/>
+    <row r="356" ht="16.5" customHeight="1"/>
+    <row r="357" ht="16.5" customHeight="1"/>
+    <row r="358" ht="16.5" customHeight="1"/>
+    <row r="359" ht="16.5" customHeight="1"/>
+    <row r="360" ht="16.5" customHeight="1"/>
+    <row r="361" ht="16.5" customHeight="1"/>
+    <row r="362" ht="16.5" customHeight="1"/>
+    <row r="363" ht="16.5" customHeight="1"/>
+    <row r="364" ht="16.5" customHeight="1"/>
+    <row r="365" ht="16.5" customHeight="1"/>
+    <row r="366" ht="16.5" customHeight="1"/>
+    <row r="367" ht="16.5" customHeight="1"/>
+    <row r="368" ht="16.5" customHeight="1"/>
+    <row r="369" ht="16.5" customHeight="1"/>
+    <row r="370" ht="16.5" customHeight="1"/>
+    <row r="371" ht="16.5" customHeight="1"/>
+    <row r="372" ht="16.5" customHeight="1"/>
+    <row r="373" ht="16.5" customHeight="1"/>
+    <row r="374" ht="16.5" customHeight="1"/>
+    <row r="375" ht="16.5" customHeight="1"/>
+    <row r="376" ht="16.5" customHeight="1"/>
+    <row r="377" ht="16.5" customHeight="1"/>
+    <row r="378" ht="16.5" customHeight="1"/>
+    <row r="379" ht="16.5" customHeight="1"/>
+    <row r="380" ht="16.5" customHeight="1"/>
+    <row r="381" ht="16.5" customHeight="1"/>
+    <row r="382" ht="16.5" customHeight="1"/>
+    <row r="383" ht="16.5" customHeight="1"/>
+    <row r="384" ht="16.5" customHeight="1"/>
+    <row r="385" ht="16.5" customHeight="1"/>
+    <row r="386" ht="16.5" customHeight="1"/>
+    <row r="387" ht="16.5" customHeight="1"/>
+    <row r="388" ht="16.5" customHeight="1"/>
+    <row r="389" ht="16.5" customHeight="1"/>
+    <row r="390" ht="16.5" customHeight="1"/>
+    <row r="391" ht="16.5" customHeight="1"/>
+    <row r="392" ht="16.5" customHeight="1"/>
+    <row r="393" ht="16.5" customHeight="1"/>
+    <row r="394" ht="16.5" customHeight="1"/>
+    <row r="395" ht="16.5" customHeight="1"/>
+    <row r="396" ht="16.5" customHeight="1"/>
+    <row r="397" ht="16.5" customHeight="1"/>
+    <row r="398" ht="16.5" customHeight="1"/>
+    <row r="399" ht="16.5" customHeight="1"/>
+    <row r="400" ht="16.5" customHeight="1"/>
+    <row r="401" ht="16.5" customHeight="1"/>
+    <row r="402" ht="16.5" customHeight="1"/>
+    <row r="403" ht="16.5" customHeight="1"/>
+    <row r="404" ht="16.5" customHeight="1"/>
+    <row r="405" ht="16.5" customHeight="1"/>
+    <row r="406" ht="16.5" customHeight="1"/>
+    <row r="407" ht="16.5" customHeight="1"/>
+    <row r="408" ht="16.5" customHeight="1"/>
+    <row r="409" ht="16.5" customHeight="1"/>
+    <row r="410" ht="16.5" customHeight="1"/>
+    <row r="411" ht="16.5" customHeight="1"/>
+    <row r="412" ht="16.5" customHeight="1"/>
+    <row r="413" ht="16.5" customHeight="1"/>
+    <row r="414" ht="16.5" customHeight="1"/>
+    <row r="415" ht="16.5" customHeight="1"/>
+    <row r="416" ht="16.5" customHeight="1"/>
+    <row r="417" ht="16.5" customHeight="1"/>
+    <row r="418" ht="16.5" customHeight="1"/>
+    <row r="419" ht="16.5" customHeight="1"/>
+    <row r="420" ht="16.5" customHeight="1"/>
+    <row r="421" ht="16.5" customHeight="1"/>
+    <row r="422" ht="16.5" customHeight="1"/>
+    <row r="423" ht="16.5" customHeight="1"/>
+    <row r="424" ht="16.5" customHeight="1"/>
+    <row r="425" ht="16.5" customHeight="1"/>
+    <row r="426" ht="16.5" customHeight="1"/>
+    <row r="427" ht="16.5" customHeight="1"/>
+    <row r="428" ht="16.5" customHeight="1"/>
+    <row r="429" ht="16.5" customHeight="1"/>
+    <row r="430" ht="16.5" customHeight="1"/>
+    <row r="431" ht="16.5" customHeight="1"/>
+    <row r="432" ht="16.5" customHeight="1"/>
+    <row r="433" ht="16.5" customHeight="1"/>
+    <row r="434" ht="16.5" customHeight="1"/>
+    <row r="435" ht="16.5" customHeight="1"/>
+    <row r="436" ht="16.5" customHeight="1"/>
+    <row r="437" ht="16.5" customHeight="1"/>
+    <row r="438" ht="16.5" customHeight="1"/>
+    <row r="439" ht="16.5" customHeight="1"/>
+    <row r="440" ht="16.5" customHeight="1"/>
+    <row r="441" ht="16.5" customHeight="1"/>
+    <row r="442" ht="16.5" customHeight="1"/>
+    <row r="443" ht="16.5" customHeight="1"/>
+    <row r="444" ht="16.5" customHeight="1"/>
+    <row r="445" ht="16.5" customHeight="1"/>
+    <row r="446" ht="16.5" customHeight="1"/>
+    <row r="447" ht="16.5" customHeight="1"/>
+    <row r="448" ht="16.5" customHeight="1"/>
+    <row r="449" ht="16.5" customHeight="1"/>
+    <row r="450" ht="16.5" customHeight="1"/>
+    <row r="451" ht="16.5" customHeight="1"/>
+    <row r="452" ht="16.5" customHeight="1"/>
+    <row r="453" ht="16.5" customHeight="1"/>
+    <row r="454" ht="16.5" customHeight="1"/>
+    <row r="455" ht="16.5" customHeight="1"/>
+    <row r="456" ht="16.5" customHeight="1"/>
+    <row r="457" ht="16.5" customHeight="1"/>
+    <row r="458" ht="16.5" customHeight="1"/>
+    <row r="459" ht="16.5" customHeight="1"/>
+    <row r="460" ht="16.5" customHeight="1"/>
+    <row r="461" ht="16.5" customHeight="1"/>
+    <row r="462" ht="16.5" customHeight="1"/>
+    <row r="463" ht="16.5" customHeight="1"/>
+    <row r="464" ht="16.5" customHeight="1"/>
+    <row r="465" ht="16.5" customHeight="1"/>
+    <row r="466" ht="16.5" customHeight="1"/>
+    <row r="467" ht="16.5" customHeight="1"/>
+    <row r="468" ht="16.5" customHeight="1"/>
+    <row r="469" ht="16.5" customHeight="1"/>
+    <row r="470" ht="16.5" customHeight="1"/>
+    <row r="471" ht="16.5" customHeight="1"/>
+    <row r="472" ht="16.5" customHeight="1"/>
+    <row r="473" ht="16.5" customHeight="1"/>
+    <row r="474" ht="16.5" customHeight="1"/>
+    <row r="475" ht="16.5" customHeight="1"/>
+    <row r="476" ht="16.5" customHeight="1"/>
+    <row r="477" ht="16.5" customHeight="1"/>
+    <row r="478" ht="16.5" customHeight="1"/>
+    <row r="479" ht="16.5" customHeight="1"/>
+    <row r="480" ht="16.5" customHeight="1"/>
+    <row r="481" ht="16.5" customHeight="1"/>
+    <row r="482" ht="16.5" customHeight="1"/>
+    <row r="483" ht="16.5" customHeight="1"/>
+    <row r="484" ht="16.5" customHeight="1"/>
+    <row r="485" ht="16.5" customHeight="1"/>
+    <row r="486" ht="16.5" customHeight="1"/>
+    <row r="487" ht="16.5" customHeight="1"/>
+    <row r="488" ht="16.5" customHeight="1"/>
+    <row r="489" ht="16.5" customHeight="1"/>
+    <row r="490" ht="16.5" customHeight="1"/>
+    <row r="491" ht="16.5" customHeight="1"/>
+    <row r="492" ht="16.5" customHeight="1"/>
+    <row r="493" ht="16.5" customHeight="1"/>
+    <row r="494" ht="16.5" customHeight="1"/>
+    <row r="495" ht="16.5" customHeight="1"/>
+    <row r="496" ht="16.5" customHeight="1"/>
+    <row r="497" ht="16.5" customHeight="1"/>
+    <row r="498" ht="16.5" customHeight="1"/>
+    <row r="499" ht="16.5" customHeight="1"/>
+    <row r="500" ht="16.5" customHeight="1"/>
+    <row r="501" ht="16.5" customHeight="1"/>
+    <row r="502" ht="16.5" customHeight="1"/>
+    <row r="503" ht="16.5" customHeight="1"/>
+    <row r="504" ht="16.5" customHeight="1"/>
+    <row r="505" ht="16.5" customHeight="1"/>
+    <row r="506" ht="16.5" customHeight="1"/>
+    <row r="507" ht="16.5" customHeight="1"/>
+    <row r="508" ht="16.5" customHeight="1"/>
+    <row r="509" ht="16.5" customHeight="1"/>
+    <row r="510" ht="16.5" customHeight="1"/>
+    <row r="511" ht="16.5" customHeight="1"/>
+    <row r="512" ht="16.5" customHeight="1"/>
+    <row r="513" ht="16.5" customHeight="1"/>
+    <row r="514" ht="16.5" customHeight="1"/>
+    <row r="515" ht="16.5" customHeight="1"/>
+    <row r="516" ht="16.5" customHeight="1"/>
+    <row r="517" ht="16.5" customHeight="1"/>
+    <row r="518" ht="16.5" customHeight="1"/>
+    <row r="519" ht="16.5" customHeight="1"/>
+    <row r="520" ht="16.5" customHeight="1"/>
+    <row r="521" ht="16.5" customHeight="1"/>
+    <row r="522" ht="16.5" customHeight="1"/>
+    <row r="523" ht="16.5" customHeight="1"/>
+    <row r="524" ht="16.5" customHeight="1"/>
+    <row r="525" ht="16.5" customHeight="1"/>
+    <row r="526" ht="16.5" customHeight="1"/>
+    <row r="527" ht="16.5" customHeight="1"/>
+    <row r="528" ht="16.5" customHeight="1"/>
+    <row r="529" ht="16.5" customHeight="1"/>
+    <row r="530" ht="16.5" customHeight="1"/>
+    <row r="531" ht="16.5" customHeight="1"/>
+    <row r="532" ht="16.5" customHeight="1"/>
+    <row r="533" ht="16.5" customHeight="1"/>
+    <row r="534" ht="16.5" customHeight="1"/>
+    <row r="535" ht="16.5" customHeight="1"/>
+    <row r="536" ht="16.5" customHeight="1"/>
+    <row r="537" ht="16.5" customHeight="1"/>
+    <row r="538" ht="16.5" customHeight="1"/>
+    <row r="539" ht="16.5" customHeight="1"/>
+    <row r="540" ht="16.5" customHeight="1"/>
+    <row r="541" ht="16.5" customHeight="1"/>
+    <row r="542" ht="16.5" customHeight="1"/>
+    <row r="543" ht="16.5" customHeight="1"/>
+    <row r="544" ht="16.5" customHeight="1"/>
+    <row r="545" ht="16.5" customHeight="1"/>
+    <row r="546" ht="16.5" customHeight="1"/>
+    <row r="547" ht="16.5" customHeight="1"/>
+    <row r="548" ht="16.5" customHeight="1"/>
+    <row r="549" ht="16.5" customHeight="1"/>
+    <row r="550" ht="16.5" customHeight="1"/>
+    <row r="551" ht="16.5" customHeight="1"/>
+    <row r="552" ht="16.5" customHeight="1"/>
+    <row r="553" ht="16.5" customHeight="1"/>
+    <row r="554" ht="16.5" customHeight="1"/>
+    <row r="555" ht="16.5" customHeight="1"/>
+    <row r="556" ht="16.5" customHeight="1"/>
+    <row r="557" ht="16.5" customHeight="1"/>
+    <row r="558" ht="16.5" customHeight="1"/>
+    <row r="559" ht="16.5" customHeight="1"/>
+    <row r="560" ht="16.5" customHeight="1"/>
+    <row r="561" ht="16.5" customHeight="1"/>
+    <row r="562" ht="16.5" customHeight="1"/>
+    <row r="563" ht="16.5" customHeight="1"/>
+    <row r="564" ht="16.5" customHeight="1"/>
+    <row r="565" ht="16.5" customHeight="1"/>
+    <row r="566" ht="16.5" customHeight="1"/>
+    <row r="567" ht="16.5" customHeight="1"/>
+    <row r="568" ht="16.5" customHeight="1"/>
+    <row r="569" ht="16.5" customHeight="1"/>
+    <row r="570" ht="16.5" customHeight="1"/>
+    <row r="571" ht="16.5" customHeight="1"/>
+    <row r="572" ht="16.5" customHeight="1"/>
+    <row r="573" ht="16.5" customHeight="1"/>
+    <row r="574" ht="16.5" customHeight="1"/>
+    <row r="575" ht="16.5" customHeight="1"/>
+    <row r="576" ht="16.5" customHeight="1"/>
+    <row r="577" ht="16.5" customHeight="1"/>
+    <row r="578" ht="16.5" customHeight="1"/>
+    <row r="579" ht="16.5" customHeight="1"/>
+    <row r="580" ht="16.5" customHeight="1"/>
+    <row r="581" ht="16.5" customHeight="1"/>
+    <row r="582" ht="16.5" customHeight="1"/>
+    <row r="583" ht="16.5" customHeight="1"/>
+    <row r="584" ht="16.5" customHeight="1"/>
+    <row r="585" ht="16.5" customHeight="1"/>
+    <row r="586" ht="16.5" customHeight="1"/>
+    <row r="587" ht="16.5" customHeight="1"/>
+    <row r="588" ht="16.5" customHeight="1"/>
+    <row r="589" ht="16.5" customHeight="1"/>
+    <row r="590" ht="16.5" customHeight="1"/>
+    <row r="591" ht="16.5" customHeight="1"/>
+    <row r="592" ht="16.5" customHeight="1"/>
+    <row r="593" ht="16.5" customHeight="1"/>
+    <row r="594" ht="16.5" customHeight="1"/>
+    <row r="595" ht="16.5" customHeight="1"/>
+    <row r="596" ht="16.5" customHeight="1"/>
+    <row r="597" ht="16.5" customHeight="1"/>
+    <row r="598" ht="16.5" customHeight="1"/>
+    <row r="599" ht="16.5" customHeight="1"/>
+    <row r="600" ht="16.5" customHeight="1"/>
+    <row r="601" ht="16.5" customHeight="1"/>
+    <row r="602" ht="16.5" customHeight="1"/>
+    <row r="603" ht="16.5" customHeight="1"/>
+    <row r="604" ht="16.5" customHeight="1"/>
+    <row r="605" ht="16.5" customHeight="1"/>
+    <row r="606" ht="16.5" customHeight="1"/>
+    <row r="607" ht="16.5" customHeight="1"/>
+    <row r="608" ht="16.5" customHeight="1"/>
+    <row r="609" ht="16.5" customHeight="1"/>
+    <row r="610" ht="16.5" customHeight="1"/>
+    <row r="611" ht="16.5" customHeight="1"/>
+    <row r="612" ht="16.5" customHeight="1"/>
+    <row r="613" ht="16.5" customHeight="1"/>
+    <row r="614" ht="16.5" customHeight="1"/>
+    <row r="615" ht="16.5" customHeight="1"/>
+    <row r="616" ht="16.5" customHeight="1"/>
+    <row r="617" ht="16.5" customHeight="1"/>
+    <row r="618" ht="16.5" customHeight="1"/>
+    <row r="619" ht="16.5" customHeight="1"/>
+    <row r="620" ht="16.5" customHeight="1"/>
+    <row r="621" ht="16.5" customHeight="1"/>
+    <row r="622" ht="16.5" customHeight="1"/>
+    <row r="623" ht="16.5" customHeight="1"/>
+    <row r="624" ht="16.5" customHeight="1"/>
+    <row r="625" ht="16.5" customHeight="1"/>
+    <row r="626" ht="16.5" customHeight="1"/>
+    <row r="627" ht="16.5" customHeight="1"/>
+    <row r="628" ht="16.5" customHeight="1"/>
+    <row r="629" ht="16.5" customHeight="1"/>
+    <row r="630" ht="16.5" customHeight="1"/>
+    <row r="631" ht="16.5" customHeight="1"/>
+    <row r="632" ht="16.5" customHeight="1"/>
+    <row r="633" ht="16.5" customHeight="1"/>
+    <row r="634" ht="16.5" customHeight="1"/>
+    <row r="635" ht="16.5" customHeight="1"/>
+    <row r="636" ht="16.5" customHeight="1"/>
+    <row r="637" ht="16.5" customHeight="1"/>
+    <row r="638" ht="16.5" customHeight="1"/>
+    <row r="639" ht="16.5" customHeight="1"/>
+    <row r="640" ht="16.5" customHeight="1"/>
+    <row r="641" ht="16.5" customHeight="1"/>
+    <row r="642" ht="16.5" customHeight="1"/>
+    <row r="643" ht="16.5" customHeight="1"/>
+    <row r="644" ht="16.5" customHeight="1"/>
+    <row r="645" ht="16.5" customHeight="1"/>
+    <row r="646" ht="16.5" customHeight="1"/>
+    <row r="647" ht="16.5" customHeight="1"/>
+    <row r="648" ht="16.5" customHeight="1"/>
+    <row r="649" ht="16.5" customHeight="1"/>
+    <row r="650" ht="16.5" customHeight="1"/>
+    <row r="651" ht="16.5" customHeight="1"/>
+    <row r="652" ht="16.5" customHeight="1"/>
+    <row r="653" ht="16.5" customHeight="1"/>
+    <row r="654" ht="16.5" customHeight="1"/>
+    <row r="655" ht="16.5" customHeight="1"/>
+    <row r="656" ht="16.5" customHeight="1"/>
+    <row r="657" ht="16.5" customHeight="1"/>
+    <row r="658" ht="16.5" customHeight="1"/>
+    <row r="659" ht="16.5" customHeight="1"/>
+    <row r="660" ht="16.5" customHeight="1"/>
+    <row r="661" ht="16.5" customHeight="1"/>
+    <row r="662" ht="16.5" customHeight="1"/>
+    <row r="663" ht="16.5" customHeight="1"/>
+    <row r="664" ht="16.5" customHeight="1"/>
+    <row r="665" ht="16.5" customHeight="1"/>
+    <row r="666" ht="16.5" customHeight="1"/>
+    <row r="667" ht="16.5" customHeight="1"/>
+    <row r="668" ht="16.5" customHeight="1"/>
+    <row r="669" ht="16.5" customHeight="1"/>
+    <row r="670" ht="16.5" customHeight="1"/>
+    <row r="671" ht="16.5" customHeight="1"/>
+    <row r="672" ht="16.5" customHeight="1"/>
+    <row r="673" ht="16.5" customHeight="1"/>
+    <row r="674" ht="16.5" customHeight="1"/>
+    <row r="675" ht="16.5" customHeight="1"/>
+    <row r="676" ht="16.5" customHeight="1"/>
+    <row r="677" ht="16.5" customHeight="1"/>
+    <row r="678" ht="16.5" customHeight="1"/>
+    <row r="679" ht="16.5" customHeight="1"/>
+    <row r="680" ht="16.5" customHeight="1"/>
+    <row r="681" ht="16.5" customHeight="1"/>
+    <row r="682" ht="16.5" customHeight="1"/>
+    <row r="683" ht="16.5" customHeight="1"/>
+    <row r="684" ht="16.5" customHeight="1"/>
+    <row r="685" ht="16.5" customHeight="1"/>
+    <row r="686" ht="16.5" customHeight="1"/>
+    <row r="687" ht="16.5" customHeight="1"/>
+    <row r="688" ht="16.5" customHeight="1"/>
+    <row r="689" ht="16.5" customHeight="1"/>
+    <row r="690" ht="16.5" customHeight="1"/>
+    <row r="691" ht="16.5" customHeight="1"/>
+    <row r="692" ht="16.5" customHeight="1"/>
+    <row r="693" ht="16.5" customHeight="1"/>
+    <row r="694" ht="16.5" customHeight="1"/>
+    <row r="695" ht="16.5" customHeight="1"/>
+    <row r="696" ht="16.5" customHeight="1"/>
+    <row r="697" ht="16.5" customHeight="1"/>
+    <row r="698" ht="16.5" customHeight="1"/>
+    <row r="699" ht="16.5" customHeight="1"/>
+    <row r="700" ht="16.5" customHeight="1"/>
+    <row r="701" ht="16.5" customHeight="1"/>
+    <row r="702" ht="16.5" customHeight="1"/>
+    <row r="703" ht="16.5" customHeight="1"/>
+    <row r="704" ht="16.5" customHeight="1"/>
+    <row r="705" ht="16.5" customHeight="1"/>
+    <row r="706" ht="16.5" customHeight="1"/>
+    <row r="707" ht="16.5" customHeight="1"/>
+    <row r="708" ht="16.5" customHeight="1"/>
+    <row r="709" ht="16.5" customHeight="1"/>
+    <row r="710" ht="16.5" customHeight="1"/>
+    <row r="711" ht="16.5" customHeight="1"/>
+    <row r="712" ht="16.5" customHeight="1"/>
+    <row r="713" ht="16.5" customHeight="1"/>
+    <row r="714" ht="16.5" customHeight="1"/>
+    <row r="715" ht="16.5" customHeight="1"/>
+    <row r="716" ht="16.5" customHeight="1"/>
+    <row r="717" ht="16.5" customHeight="1"/>
+    <row r="718" ht="16.5" customHeight="1"/>
+    <row r="719" ht="16.5" customHeight="1"/>
+    <row r="720" ht="16.5" customHeight="1"/>
+    <row r="721" ht="16.5" customHeight="1"/>
+    <row r="722" ht="16.5" customHeight="1"/>
+    <row r="723" ht="16.5" customHeight="1"/>
+    <row r="724" ht="16.5" customHeight="1"/>
+    <row r="725" ht="16.5" customHeight="1"/>
+    <row r="726" ht="16.5" customHeight="1"/>
+    <row r="727" ht="16.5" customHeight="1"/>
+    <row r="728" ht="16.5" customHeight="1"/>
+    <row r="729" ht="16.5" customHeight="1"/>
+    <row r="730" ht="16.5" customHeight="1"/>
+    <row r="731" ht="16.5" customHeight="1"/>
+    <row r="732" ht="16.5" customHeight="1"/>
+    <row r="733" ht="16.5" customHeight="1"/>
+    <row r="734" ht="16.5" customHeight="1"/>
+    <row r="735" ht="16.5" customHeight="1"/>
+    <row r="736" ht="16.5" customHeight="1"/>
+    <row r="737" ht="16.5" customHeight="1"/>
+    <row r="738" ht="16.5" customHeight="1"/>
+    <row r="739" ht="16.5" customHeight="1"/>
+    <row r="740" ht="16.5" customHeight="1"/>
+    <row r="741" ht="16.5" customHeight="1"/>
+    <row r="742" ht="16.5" customHeight="1"/>
+    <row r="743" ht="16.5" customHeight="1"/>
+    <row r="744" ht="16.5" customHeight="1"/>
+    <row r="745" ht="16.5" customHeight="1"/>
+    <row r="746" ht="16.5" customHeight="1"/>
+    <row r="747" ht="16.5" customHeight="1"/>
+    <row r="748" ht="16.5" customHeight="1"/>
+    <row r="749" ht="16.5" customHeight="1"/>
+    <row r="750" ht="16.5" customHeight="1"/>
+    <row r="751" ht="16.5" customHeight="1"/>
+    <row r="752" ht="16.5" customHeight="1"/>
+    <row r="753" ht="16.5" customHeight="1"/>
+    <row r="754" ht="16.5" customHeight="1"/>
+    <row r="755" ht="16.5" customHeight="1"/>
+    <row r="756" ht="16.5" customHeight="1"/>
+    <row r="757" ht="16.5" customHeight="1"/>
+    <row r="758" ht="16.5" customHeight="1"/>
+    <row r="759" ht="16.5" customHeight="1"/>
+    <row r="760" ht="16.5" customHeight="1"/>
+    <row r="761" ht="16.5" customHeight="1"/>
+    <row r="762" ht="16.5" customHeight="1"/>
+    <row r="763" ht="16.5" customHeight="1"/>
+    <row r="764" ht="16.5" customHeight="1"/>
+    <row r="765" ht="16.5" customHeight="1"/>
+    <row r="766" ht="16.5" customHeight="1"/>
+    <row r="767" ht="16.5" customHeight="1"/>
+    <row r="768" ht="16.5" customHeight="1"/>
+    <row r="769" ht="16.5" customHeight="1"/>
+    <row r="770" ht="16.5" customHeight="1"/>
+    <row r="771" ht="16.5" customHeight="1"/>
+    <row r="772" ht="16.5" customHeight="1"/>
+    <row r="773" ht="16.5" customHeight="1"/>
+    <row r="774" ht="16.5" customHeight="1"/>
+    <row r="775" ht="16.5" customHeight="1"/>
+    <row r="776" ht="16.5" customHeight="1"/>
+    <row r="777" ht="16.5" customHeight="1"/>
+    <row r="778" ht="16.5" customHeight="1"/>
+    <row r="779" ht="16.5" customHeight="1"/>
+    <row r="780" ht="16.5" customHeight="1"/>
+    <row r="781" ht="16.5" customHeight="1"/>
+    <row r="782" ht="16.5" customHeight="1"/>
+    <row r="783" ht="16.5" customHeight="1"/>
+    <row r="784" ht="16.5" customHeight="1"/>
+    <row r="785" ht="16.5" customHeight="1"/>
+    <row r="786" ht="16.5" customHeight="1"/>
+    <row r="787" ht="16.5" customHeight="1"/>
+    <row r="788" ht="16.5" customHeight="1"/>
+    <row r="789" ht="16.5" customHeight="1"/>
+    <row r="790" ht="16.5" customHeight="1"/>
+    <row r="791" ht="16.5" customHeight="1"/>
+    <row r="792" ht="16.5" customHeight="1"/>
+    <row r="793" ht="16.5" customHeight="1"/>
+    <row r="794" ht="16.5" customHeight="1"/>
+    <row r="795" ht="16.5" customHeight="1"/>
+    <row r="796" ht="16.5" customHeight="1"/>
+    <row r="797" ht="16.5" customHeight="1"/>
+    <row r="798" ht="16.5" customHeight="1"/>
+    <row r="799" ht="16.5" customHeight="1"/>
+    <row r="800" ht="16.5" customHeight="1"/>
+    <row r="801" ht="16.5" customHeight="1"/>
+    <row r="802" ht="16.5" customHeight="1"/>
+    <row r="803" ht="16.5" customHeight="1"/>
+    <row r="804" ht="16.5" customHeight="1"/>
+    <row r="805" ht="16.5" customHeight="1"/>
+    <row r="806" ht="16.5" customHeight="1"/>
+    <row r="807" ht="16.5" customHeight="1"/>
+    <row r="808" ht="16.5" customHeight="1"/>
+    <row r="809" ht="16.5" customHeight="1"/>
+    <row r="810" ht="16.5" customHeight="1"/>
+    <row r="811" ht="16.5" customHeight="1"/>
+    <row r="812" ht="16.5" customHeight="1"/>
+    <row r="813" ht="16.5" customHeight="1"/>
+    <row r="814" ht="16.5" customHeight="1"/>
+    <row r="815" ht="16.5" customHeight="1"/>
+    <row r="816" ht="16.5" customHeight="1"/>
+    <row r="817" ht="16.5" customHeight="1"/>
+    <row r="818" ht="16.5" customHeight="1"/>
+    <row r="819" ht="16.5" customHeight="1"/>
+    <row r="820" ht="16.5" customHeight="1"/>
+    <row r="821" ht="16.5" customHeight="1"/>
+    <row r="822" ht="16.5" customHeight="1"/>
+    <row r="823" ht="16.5" customHeight="1"/>
+    <row r="824" ht="16.5" customHeight="1"/>
+    <row r="825" ht="16.5" customHeight="1"/>
+    <row r="826" ht="16.5" customHeight="1"/>
+    <row r="827" ht="16.5" customHeight="1"/>
+    <row r="828" ht="16.5" customHeight="1"/>
+    <row r="829" ht="16.5" customHeight="1"/>
+    <row r="830" ht="16.5" customHeight="1"/>
+    <row r="831" ht="16.5" customHeight="1"/>
+    <row r="832" ht="16.5" customHeight="1"/>
+    <row r="833" ht="16.5" customHeight="1"/>
+    <row r="834" ht="16.5" customHeight="1"/>
+    <row r="835" ht="16.5" customHeight="1"/>
+    <row r="836" ht="16.5" customHeight="1"/>
+    <row r="837" ht="16.5" customHeight="1"/>
+    <row r="838" ht="16.5" customHeight="1"/>
+    <row r="839" ht="16.5" customHeight="1"/>
+    <row r="840" ht="16.5" customHeight="1"/>
+    <row r="841" ht="16.5" customHeight="1"/>
+    <row r="842" ht="16.5" customHeight="1"/>
+    <row r="843" ht="16.5" customHeight="1"/>
+    <row r="844" ht="16.5" customHeight="1"/>
+    <row r="845" ht="16.5" customHeight="1"/>
+    <row r="846" ht="16.5" customHeight="1"/>
+    <row r="847" ht="16.5" customHeight="1"/>
+    <row r="848" ht="16.5" customHeight="1"/>
+    <row r="849" ht="16.5" customHeight="1"/>
+    <row r="850" ht="16.5" customHeight="1"/>
+    <row r="851" ht="16.5" customHeight="1"/>
+    <row r="852" ht="16.5" customHeight="1"/>
+    <row r="853" ht="16.5" customHeight="1"/>
+    <row r="854" ht="16.5" customHeight="1"/>
+    <row r="855" ht="16.5" customHeight="1"/>
+    <row r="856" ht="16.5" customHeight="1"/>
+    <row r="857" ht="16.5" customHeight="1"/>
+    <row r="858" ht="16.5" customHeight="1"/>
+    <row r="859" ht="16.5" customHeight="1"/>
+    <row r="860" ht="16.5" customHeight="1"/>
+    <row r="861" ht="16.5" customHeight="1"/>
+    <row r="862" ht="16.5" customHeight="1"/>
+    <row r="863" ht="16.5" customHeight="1"/>
+    <row r="864" ht="16.5" customHeight="1"/>
+    <row r="865" ht="16.5" customHeight="1"/>
+    <row r="866" ht="16.5" customHeight="1"/>
+    <row r="867" ht="16.5" customHeight="1"/>
+    <row r="868" ht="16.5" customHeight="1"/>
+    <row r="869" ht="16.5" customHeight="1"/>
+    <row r="870" ht="16.5" customHeight="1"/>
+    <row r="871" ht="16.5" customHeight="1"/>
+    <row r="872" ht="16.5" customHeight="1"/>
+    <row r="873" ht="16.5" customHeight="1"/>
+    <row r="874" ht="16.5" customHeight="1"/>
+    <row r="875" ht="16.5" customHeight="1"/>
+    <row r="876" ht="16.5" customHeight="1"/>
+    <row r="877" ht="16.5" customHeight="1"/>
+    <row r="878" ht="16.5" customHeight="1"/>
+    <row r="879" ht="16.5" customHeight="1"/>
+    <row r="880" ht="16.5" customHeight="1"/>
+    <row r="881" ht="16.5" customHeight="1"/>
+    <row r="882" ht="16.5" customHeight="1"/>
+    <row r="883" ht="16.5" customHeight="1"/>
+    <row r="884" ht="16.5" customHeight="1"/>
+    <row r="885" ht="16.5" customHeight="1"/>
+    <row r="886" ht="16.5" customHeight="1"/>
+    <row r="887" ht="16.5" customHeight="1"/>
+    <row r="888" ht="16.5" customHeight="1"/>
+    <row r="889" ht="16.5" customHeight="1"/>
+    <row r="890" ht="16.5" customHeight="1"/>
+    <row r="891" ht="16.5" customHeight="1"/>
+    <row r="892" ht="16.5" customHeight="1"/>
+    <row r="893" ht="16.5" customHeight="1"/>
+    <row r="894" ht="16.5" customHeight="1"/>
+    <row r="895" ht="16.5" customHeight="1"/>
+    <row r="896" ht="16.5" customHeight="1"/>
+    <row r="897" ht="16.5" customHeight="1"/>
+    <row r="898" ht="16.5" customHeight="1"/>
+    <row r="899" ht="16.5" customHeight="1"/>
+    <row r="900" ht="16.5" customHeight="1"/>
+    <row r="901" ht="16.5" customHeight="1"/>
+    <row r="902" ht="16.5" customHeight="1"/>
+    <row r="903" ht="16.5" customHeight="1"/>
+    <row r="904" ht="16.5" customHeight="1"/>
+    <row r="905" ht="16.5" customHeight="1"/>
+    <row r="906" ht="16.5" customHeight="1"/>
+    <row r="907" ht="16.5" customHeight="1"/>
+    <row r="908" ht="16.5" customHeight="1"/>
+    <row r="909" ht="16.5" customHeight="1"/>
+    <row r="910" ht="16.5" customHeight="1"/>
+    <row r="911" ht="16.5" customHeight="1"/>
+    <row r="912" ht="16.5" customHeight="1"/>
+    <row r="913" ht="16.5" customHeight="1"/>
+    <row r="914" ht="16.5" customHeight="1"/>
+    <row r="915" ht="16.5" customHeight="1"/>
+    <row r="916" ht="16.5" customHeight="1"/>
+    <row r="917" ht="16.5" customHeight="1"/>
+    <row r="918" ht="16.5" customHeight="1"/>
+    <row r="919" ht="16.5" customHeight="1"/>
+    <row r="920" ht="16.5" customHeight="1"/>
+    <row r="921" ht="16.5" customHeight="1"/>
+    <row r="922" ht="16.5" customHeight="1"/>
+    <row r="923" ht="16.5" customHeight="1"/>
+    <row r="924" ht="16.5" customHeight="1"/>
+    <row r="925" ht="16.5" customHeight="1"/>
+    <row r="926" ht="16.5" customHeight="1"/>
+    <row r="927" ht="16.5" customHeight="1"/>
+    <row r="928" ht="16.5" customHeight="1"/>
+    <row r="929" ht="16.5" customHeight="1"/>
+    <row r="930" ht="16.5" customHeight="1"/>
+    <row r="931" ht="16.5" customHeight="1"/>
+    <row r="932" ht="16.5" customHeight="1"/>
+    <row r="933" ht="16.5" customHeight="1"/>
+    <row r="934" ht="16.5" customHeight="1"/>
+    <row r="935" ht="16.5" customHeight="1"/>
+    <row r="936" ht="16.5" customHeight="1"/>
+    <row r="937" ht="16.5" customHeight="1"/>
+    <row r="938" ht="16.5" customHeight="1"/>
+    <row r="939" ht="16.5" customHeight="1"/>
+    <row r="940" ht="16.5" customHeight="1"/>
+    <row r="941" ht="16.5" customHeight="1"/>
+    <row r="942" ht="16.5" customHeight="1"/>
+    <row r="943" ht="16.5" customHeight="1"/>
+    <row r="944" ht="16.5" customHeight="1"/>
+    <row r="945" ht="16.5" customHeight="1"/>
+    <row r="946" ht="16.5" customHeight="1"/>
+    <row r="947" ht="16.5" customHeight="1"/>
+    <row r="948" ht="16.5" customHeight="1"/>
+    <row r="949" ht="16.5" customHeight="1"/>
+    <row r="950" ht="16.5" customHeight="1"/>
+    <row r="951" ht="16.5" customHeight="1"/>
+    <row r="952" ht="16.5" customHeight="1"/>
+    <row r="953" ht="16.5" customHeight="1"/>
+    <row r="954" ht="16.5" customHeight="1"/>
+    <row r="955" ht="16.5" customHeight="1"/>
+    <row r="956" ht="16.5" customHeight="1"/>
+    <row r="957" ht="16.5" customHeight="1"/>
+    <row r="958" ht="16.5" customHeight="1"/>
+    <row r="959" ht="16.5" customHeight="1"/>
+    <row r="960" ht="16.5" customHeight="1"/>
+    <row r="961" ht="16.5" customHeight="1"/>
+    <row r="962" ht="16.5" customHeight="1"/>
+    <row r="963" ht="16.5" customHeight="1"/>
+    <row r="964" ht="16.5" customHeight="1"/>
+    <row r="965" ht="16.5" customHeight="1"/>
+    <row r="966" ht="16.5" customHeight="1"/>
+    <row r="967" ht="16.5" customHeight="1"/>
+    <row r="968" ht="16.5" customHeight="1"/>
+    <row r="969" ht="16.5" customHeight="1"/>
+    <row r="970" ht="16.5" customHeight="1"/>
+    <row r="971" ht="16.5" customHeight="1"/>
+    <row r="972" ht="16.5" customHeight="1"/>
+    <row r="973" ht="16.5" customHeight="1"/>
+    <row r="974" ht="16.5" customHeight="1"/>
+    <row r="975" ht="16.5" customHeight="1"/>
+    <row r="976" ht="16.5" customHeight="1"/>
+    <row r="977" ht="16.5" customHeight="1"/>
+    <row r="978" ht="16.5" customHeight="1"/>
+    <row r="979" ht="16.5" customHeight="1"/>
+    <row r="980" ht="16.5" customHeight="1"/>
+    <row r="981" ht="16.5" customHeight="1"/>
+    <row r="982" ht="16.5" customHeight="1"/>
+    <row r="983" ht="16.5" customHeight="1"/>
+    <row r="984" ht="16.5" customHeight="1"/>
+    <row r="985" ht="16.5" customHeight="1"/>
+    <row r="986" ht="16.5" customHeight="1"/>
+    <row r="987" ht="16.5" customHeight="1"/>
+    <row r="988" ht="16.5" customHeight="1"/>
+    <row r="989" ht="16.5" customHeight="1"/>
+    <row r="990" ht="16.5" customHeight="1"/>
+    <row r="991" ht="16.5" customHeight="1"/>
+    <row r="992" ht="16.5" customHeight="1"/>
+    <row r="993" ht="16.5" customHeight="1"/>
+    <row r="994" ht="16.5" customHeight="1"/>
+    <row r="995" ht="16.5" customHeight="1"/>
+    <row r="996" ht="16.5" customHeight="1"/>
+    <row r="997" ht="16.5" customHeight="1"/>
+    <row r="998" ht="16.5" customHeight="1"/>
+    <row r="999" ht="16.5" customHeight="1"/>
+    <row r="1000" ht="16.5" customHeight="1"/>
+    <row r="1001" ht="16.5" customHeight="1"/>
+    <row r="1002" ht="16.5" customHeight="1"/>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>